<commit_message>
Added if statements to not write to excel file or try to do calculations if there are anything other than 2 saved frames
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>TrunkROM</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>AnkleROM</t>
+  </si>
+  <si>
+    <t>You need two saved frames</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,6 +416,20 @@
         <v>27.52047729492188</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added functionality to specify more than one joint you are looking for
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,6 +430,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <v>30.15035247802734</v>
+      </c>
+      <c r="C5">
+        <v>61.42125701904297</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more joints including shoulder flexion and reorganized keypoints.py so its less messy
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -14,21 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TrunkROM</t>
   </si>
   <si>
-    <t>HipROM</t>
-  </si>
-  <si>
-    <t>KneeROM</t>
+    <t>RIGHT HIP ROM</t>
+  </si>
+  <si>
+    <t>LEFT HIP ROM</t>
+  </si>
+  <si>
+    <t>RIGHT KNEE ROM</t>
+  </si>
+  <si>
+    <t>LEFT KNEE ROM</t>
   </si>
   <si>
     <t>AnkleROM</t>
   </si>
   <si>
-    <t>You need two saved frames</t>
+    <t>RIGHT SHOULDER FLEXION ROM</t>
+  </si>
+  <si>
+    <t>LEFT SHOULDER FLEXION ROM</t>
   </si>
 </sst>
 </file>
@@ -386,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,37 +414,28 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="C2">
-        <v>14.27439880371094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3">
-        <v>27.52047729492188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5">
-        <v>30.15035247802734</v>
-      </c>
-      <c r="C5">
-        <v>61.42125701904297</v>
+    <row r="2" spans="1:8">
+      <c r="B2">
+        <v>0.269439697265625</v>
+      </c>
+      <c r="D2">
+        <v>0.0922698974609375</v>
+      </c>
+      <c r="G2">
+        <v>0.9779548645019531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added an auto ID feature that counts up by one for each person
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
   <si>
     <t>TrunkROM</t>
   </si>
@@ -395,13 +401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,16 +432,61 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="D2">
         <v>0.269439697265625</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.0922698974609375</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.9779548645019531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <v>44.78070068359375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>46.16134643554688</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>40.92935180664062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rewrote Keypoints and broke it down into multiple functions
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,6 +489,28 @@
         <v>40.92935180664062</v>
       </c>
     </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>25.85023498535156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>41.47622680664062</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added vertical trunk calculation since it needs to be an absolutle angle defined by the environement (added with the conny edge detector). This also displays a level or not level text to the webcam for the relative angle
</commit_message>
<xml_diff>
--- a/ROM.xlsx
+++ b/ROM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patk1\OneDrive\Desktop\Git Hub\Joint-Angles-2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E43FBC1-8BC4-4E97-9651-E9E0C8D1B110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6285" yWindow="6510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,7 +28,7 @@
     <t>AGE</t>
   </si>
   <si>
-    <t>TrunkROM</t>
+    <t>TRUNK ROM</t>
   </si>
   <si>
     <t>RIGHT HIP ROM</t>
@@ -49,8 +55,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +119,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +171,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +205,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +240,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +416,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,13 +468,13 @@
         <v>0.269439697265625</v>
       </c>
       <c r="F2">
-        <v>0.0922698974609375</v>
+        <v>9.22698974609375E-2</v>
       </c>
       <c r="I2">
-        <v>0.9779548645019531</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>0.97795486450195313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -467,7 +485,7 @@
         <v>44.78070068359375</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -475,10 +493,10 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <v>46.16134643554688</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>46.161346435546882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -486,10 +504,10 @@
         <v>33</v>
       </c>
       <c r="F5">
-        <v>40.92935180664062</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>40.929351806640618</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -497,10 +515,10 @@
         <v>35</v>
       </c>
       <c r="F6">
-        <v>25.85023498535156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>25.850234985351559</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -508,7 +526,40 @@
         <v>28</v>
       </c>
       <c r="D7">
-        <v>41.47622680664062</v>
+        <v>41.476226806640618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>34.546051025390618</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>23.148506164550781</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>35.719680665195241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>